<commit_message>
add Read me n merge some
</commit_message>
<xml_diff>
--- a/excelOutput/33689_output.xlsx
+++ b/excelOutput/33689_output.xlsx
@@ -18,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="000000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,9 +50,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,7 +576,7 @@
     <row r="3" ht="135" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2022-05-04 10:42:32</t>
+          <t>2022-05-04 15:04:23</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -578,16 +584,16 @@
           <t>2.在右方工具列欄位雙擊筆的圖示</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>pass</t>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="4" ht="135" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2022-05-04 10:42:40</t>
+          <t>2022-05-04 15:04:31</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
@@ -595,16 +601,16 @@
           <t>3.在選單上方筆的種類中選取AI PEN</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>pass</t>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="5" ht="135" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2022-05-04 10:42:54</t>
+          <t>2022-05-04 15:04:45</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -612,16 +618,16 @@
           <t>4.在AI PEN視窗右側畫畫</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>pass</t>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="6" ht="135" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2022-05-04 10:43:09</t>
+          <t>2022-05-04 15:04:59</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -629,9 +635,9 @@
           <t>5.將搜尋結果拖曳至畫布上</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>pass</t>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>

</xml_diff>